<commit_message>
PROS-10763 - MARSRU - New KPIs
</commit_message>
<xml_diff>
--- a/Projects/MARSRU_PROD/Data/2019/KPIs to SQL.xlsx
+++ b/Projects/MARSRU_PROD/Data/2019/KPIs to SQL.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2108" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2164" uniqueCount="137">
   <si>
     <t xml:space="preserve">A</t>
   </si>
@@ -415,6 +415,18 @@
   </si>
   <si>
     <t xml:space="preserve">PSS Другие производители </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Выберите тип ДМП</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Проходит ли с данного дисплея промо активность?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Укажите общее количество фейсингов Марс на ДМП (кол-во фейсингов из цены мотивационная программа)</t>
   </si>
   <si>
     <t xml:space="preserve">Категория товаров для животных примыкает к ПРОМО АЛЛЕЕ, находится дальше 5-ти метров от входа и визуально доступна покупателям по ходу их движения без необходимости оборачиваться</t>
@@ -741,19 +753,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K151"/>
+  <dimension ref="A1:K156"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A121" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B151" activeCellId="0" sqref="B151"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A143" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D166" activeCellId="0" sqref="D166"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="4" min="1" style="1" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="10" min="6" style="1" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="286.454081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="1" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="19.8622448979592"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="1" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="10" min="6" style="1" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="283.34693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="1" width="10.8010204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6315,6 +6329,154 @@
       <c r="K151" s="1" t="str">
         <f aca="false">CONCATENATE(F151,E151,G151,A151,H151,A151,I151,D151,J151)</f>
         <v>('1436', NULL, '1016', '1016', '20', '3', '5', 'Custom', '3', '1', '0', '0', '0', '0', '0',NULL),</v>
+      </c>
+    </row>
+    <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A153" s="27" t="n">
+        <v>10011</v>
+      </c>
+      <c r="B153" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C153" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D153" s="1" t="str">
+        <f aca="false">IF(EXACT(C153,"Boolean"),"'10'","NULL")</f>
+        <v>NULL</v>
+      </c>
+      <c r="E153" s="1" t="n">
+        <v>1437</v>
+      </c>
+      <c r="F153" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G153" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H153" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I153" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J153" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K153" s="1" t="str">
+        <f aca="false">CONCATENATE(F153,E153,G153,A153,H153,A153,I153,D153,J153)</f>
+        <v>('1437', NULL, '10011', '10011', '20', '3', '5', 'Custom', '3', '1', '0', '0', '0', '0', '0',NULL),</v>
+      </c>
+    </row>
+    <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A154" s="27" t="n">
+        <v>10012</v>
+      </c>
+      <c r="B154" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C154" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D154" s="1" t="str">
+        <f aca="false">IF(EXACT(C154,"Boolean"),"'10'","NULL")</f>
+        <v>'10'</v>
+      </c>
+      <c r="E154" s="1" t="n">
+        <v>1438</v>
+      </c>
+      <c r="F154" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G154" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H154" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I154" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J154" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K154" s="1" t="str">
+        <f aca="false">CONCATENATE(F154,E154,G154,A154,H154,A154,I154,D154,J154)</f>
+        <v>('1438', NULL, '10012', '10012', '20', '3', '5', 'Custom', '3', '1', '0', '0', '0', '0', '0','10'),</v>
+      </c>
+    </row>
+    <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A155" s="27" t="n">
+        <v>10014</v>
+      </c>
+      <c r="B155" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C155" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D155" s="1" t="str">
+        <f aca="false">IF(EXACT(C155,"Boolean"),"'10'","NULL")</f>
+        <v>NULL</v>
+      </c>
+      <c r="E155" s="1" t="n">
+        <v>1439</v>
+      </c>
+      <c r="F155" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G155" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H155" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I155" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J155" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K155" s="1" t="str">
+        <f aca="false">CONCATENATE(F155,E155,G155,A155,H155,A155,I155,D155,J155)</f>
+        <v>('1439', NULL, '10014', '10014', '20', '3', '5', 'Custom', '3', '1', '0', '0', '0', '0', '0',NULL),</v>
+      </c>
+    </row>
+    <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A156" s="27" t="n">
+        <v>10013</v>
+      </c>
+      <c r="B156" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C156" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D156" s="1" t="str">
+        <f aca="false">IF(EXACT(C156,"Boolean"),"'10'","NULL")</f>
+        <v>NULL</v>
+      </c>
+      <c r="E156" s="1" t="n">
+        <v>1440</v>
+      </c>
+      <c r="F156" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G156" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H156" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I156" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J156" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K156" s="1" t="str">
+        <f aca="false">CONCATENATE(F156,E156,G156,A156,H156,A156,I156,D156,J156)</f>
+        <v>('1440', NULL, '10013', '10013', '20', '3', '5', 'Custom', '3', '1', '0', '0', '0', '0', '0',NULL),</v>
       </c>
     </row>
   </sheetData>
@@ -6333,17 +6495,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K151"/>
+  <dimension ref="A1:K156"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A124" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K145" activeCellId="0" sqref="K145"/>
+      <selection pane="topLeft" activeCell="B155" activeCellId="0" sqref="B155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="4" min="1" style="1" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="1" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="4" min="1" style="1" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="1" width="10.8010204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8347,7 +8509,7 @@
         <v>2219</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="C55" s="4" t="s">
         <v>20</v>
@@ -10345,7 +10507,7 @@
         <v>4219</v>
       </c>
       <c r="B109" s="21" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="C109" s="4" t="s">
         <v>20</v>
@@ -11653,7 +11815,7 @@
         <v>1010</v>
       </c>
       <c r="B145" s="28" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="C145" s="1" t="s">
         <v>12</v>
@@ -11905,6 +12067,154 @@
       <c r="K151" s="1" t="str">
         <f aca="false">CONCATENATE(F151,E151,G151,CONCATENATE(A151,"-RUS"),H151,CONCATENATE(A151," - ",B151),I151,D151,J151)</f>
         <v>('2436', NULL, '1016-RUS', '1016 - PSS Другие производители ', '20', '3', '5', 'Custom', '3', '1', '0', '0', '0', '0', '0',NULL),</v>
+      </c>
+    </row>
+    <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A153" s="27" t="n">
+        <v>10011</v>
+      </c>
+      <c r="B153" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C153" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D153" s="1" t="str">
+        <f aca="false">IF(EXACT(C153,"Boolean"),"'10'","NULL")</f>
+        <v>NULL</v>
+      </c>
+      <c r="E153" s="1" t="n">
+        <v>2732</v>
+      </c>
+      <c r="F153" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G153" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H153" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I153" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J153" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K153" s="1" t="str">
+        <f aca="false">CONCATENATE(F153,E153,G153,CONCATENATE(A153,"-RUS"),H153,CONCATENATE(A153," - ",B153),I153,D153,J153)</f>
+        <v>('2732', NULL, '10011-RUS', '10011 - Выберите тип ДМП', '20', '3', '5', 'Custom', '3', '1', '0', '0', '0', '0', '0',NULL),</v>
+      </c>
+    </row>
+    <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A154" s="27" t="n">
+        <v>10012</v>
+      </c>
+      <c r="B154" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C154" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D154" s="1" t="str">
+        <f aca="false">IF(EXACT(C154,"Boolean"),"'10'","NULL")</f>
+        <v>'10'</v>
+      </c>
+      <c r="E154" s="1" t="n">
+        <v>2733</v>
+      </c>
+      <c r="F154" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G154" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H154" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I154" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J154" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K154" s="1" t="str">
+        <f aca="false">CONCATENATE(F154,E154,G154,CONCATENATE(A154,"-RUS"),H154,CONCATENATE(A154," - ",B154),I154,D154,J154)</f>
+        <v>('2733', NULL, '10012-RUS', '10012 - Проходит ли с данного дисплея промо активность?', '20', '3', '5', 'Custom', '3', '1', '0', '0', '0', '0', '0','10'),</v>
+      </c>
+    </row>
+    <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A155" s="27" t="n">
+        <v>10014</v>
+      </c>
+      <c r="B155" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C155" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D155" s="1" t="str">
+        <f aca="false">IF(EXACT(C155,"Boolean"),"'10'","NULL")</f>
+        <v>NULL</v>
+      </c>
+      <c r="E155" s="1" t="n">
+        <v>2734</v>
+      </c>
+      <c r="F155" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G155" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H155" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I155" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J155" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K155" s="1" t="str">
+        <f aca="false">CONCATENATE(F155,E155,G155,CONCATENATE(A155,"-RUS"),H155,CONCATENATE(A155," - ",B155),I155,D155,J155)</f>
+        <v>('2734', NULL, '10014-RUS', '10014 - Укажите общее количество фейсингов Марс на ДМП (кол-во фейсингов из цены мотивационная программа)', '20', '3', '5', 'Custom', '3', '1', '0', '0', '0', '0', '0',NULL),</v>
+      </c>
+    </row>
+    <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A156" s="27" t="n">
+        <v>10013</v>
+      </c>
+      <c r="B156" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C156" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D156" s="1" t="str">
+        <f aca="false">IF(EXACT(C156,"Boolean"),"'10'","NULL")</f>
+        <v>NULL</v>
+      </c>
+      <c r="E156" s="1" t="n">
+        <v>2735</v>
+      </c>
+      <c r="F156" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G156" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H156" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I156" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J156" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K156" s="1" t="str">
+        <f aca="false">CONCATENATE(F156,E156,G156,CONCATENATE(A156,"-RUS"),H156,CONCATENATE(A156," - ",B156),I156,D156,J156)</f>
+        <v>('2735', NULL, '10013-RUS', '10013 - Выберите тип ДМП', '20', '3', '5', 'Custom', '3', '1', '0', '0', '0', '0', '0',NULL),</v>
       </c>
     </row>
   </sheetData>

</xml_diff>